<commit_message>
Actualizacion 01-06-2020 carga masiva
</commit_message>
<xml_diff>
--- a/Infatlan_STEI_Inventario/pages/plantillas/PlantillaEnlaces.xlsx
+++ b/Infatlan_STEI_Inventario/pages/plantillas/PlantillaEnlaces.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpadilla\Desktop\inventario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wpadilla\source\repos\Infatlan_STEI_Actual\Infatlan_STEI_Inventario\pages\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B32F4876-4348-49F9-9758-69B39A50109F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59A82B1-FCB3-41B4-A293-1970359E7DA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5217C7B4-8BF1-4F76-91D5-C21BB50F6256}"/>
   </bookViews>
@@ -31,9 +31,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>nombreNodo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>IP_ORIGEN</t>
+  </si>
+  <si>
+    <t>IP_DESTINO</t>
+  </si>
+  <si>
+    <t>SERVICIOS</t>
+  </si>
+  <si>
+    <t>CONTACTO</t>
+  </si>
+  <si>
+    <t>TELEFONO</t>
+  </si>
+  <si>
+    <t>ID_TIPO</t>
+  </si>
+  <si>
+    <t>ID_PROVEEDOR</t>
+  </si>
+  <si>
+    <t>ID_ORIGEN</t>
+  </si>
+  <si>
+    <t>ID_DESTINO</t>
   </si>
 </sst>
 </file>
@@ -49,6 +79,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -65,17 +96,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -84,7 +130,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,23 +445,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8E5053-7D3C-4F58-A0B9-D50C5EE5F584}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>